<commit_message>
try to add figures
</commit_message>
<xml_diff>
--- a/specifics/QM2-22-WiSe-Modulverlauf.xlsx
+++ b/specifics/QM2-22-WiSe-Modulverlauf.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiansaueruser/github-repos/start-bayes/specifics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98A52E6-8F07-4647-A422-E569C7295521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCBB9DF-0BC8-EE4F-8897-292BAB8780B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16900" xr2:uid="{B4BA407F-7EF6-F641-926D-2394B79BC202}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Nr</t>
   </si>
@@ -133,13 +133,16 @@
     <t>Globusversuch</t>
   </si>
   <si>
-    <t>Fallstudien</t>
-  </si>
-  <si>
     <t>Erster Termin: 4. Okt. 22, 14.15-15.00</t>
   </si>
   <si>
-    <t>Ab diese Woche benötigen wir rstanarm. Am Do., 3. 11. entfällt die Übung.</t>
+    <t>Ab diese Woche benötigen wir rstanarm.</t>
+  </si>
+  <si>
+    <t>Am Di., 1.11. entfällt die Vorlesung. Am Do., 3. 11. entfällt die Übung.</t>
+  </si>
+  <si>
+    <t>Aufhol-Woche</t>
   </si>
 </sst>
 </file>
@@ -503,7 +506,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,7 +541,7 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -579,7 +582,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -593,10 +596,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -615,7 +621,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
@@ -626,7 +632,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -637,7 +643,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>
@@ -648,7 +654,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>25</v>
@@ -659,7 +665,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>

</xml_diff>